<commit_message>
updated file inputs and outputs
</commit_message>
<xml_diff>
--- a/test/input_files/op1.plate_layout_to_spreadsheet/plate_spreadsheet_template.xlsx
+++ b/test/input_files/op1.plate_layout_to_spreadsheet/plate_spreadsheet_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Genomics-Metadata-Multiplexing\test\input_files\op1.plate_layout_to_spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C897A913-163F-442D-9C04-06769E55CEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BDDB54-C8F6-4943-BAB2-FDCA8BEC0C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33495" yWindow="705" windowWidth="30945" windowHeight="19470" xr2:uid="{E5692559-4AE4-9B44-98DF-B853A533C26D}"/>
+    <workbookView xWindow="-33705" yWindow="750" windowWidth="32040" windowHeight="20130" xr2:uid="{E5692559-4AE4-9B44-98DF-B853A533C26D}"/>
   </bookViews>
   <sheets>
     <sheet name="LCE123" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t xml:space="preserve">Collaboration : </t>
   </si>
@@ -122,16 +122,12 @@
     <t>Test after sort</t>
   </si>
   <si>
-    <t>SampleA</t>
-  </si>
-  <si>
-    <t>SampleB</t>
-  </si>
-  <si>
-    <t>SampleC</t>
-  </si>
-  <si>
-    <t>SampleD</t>
+    <t>NKC_084</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>NKC_085</t>
+    <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -755,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA52931-74CB-D945-A397-3D201927F083}">
   <dimension ref="A1:AD74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -1533,13 +1529,13 @@
     <row r="34" spans="1:26" ht="21.95" customHeight="1">
       <c r="A34" s="29"/>
       <c r="B34" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:26" s="21" customFormat="1" ht="21.95" customHeight="1">
       <c r="A35" s="30"/>
       <c r="B35" s="26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C35" s="31"/>
       <c r="D35" s="31"/>
@@ -1569,7 +1565,7 @@
     <row r="36" spans="1:26" s="21" customFormat="1" ht="20.25">
       <c r="A36" s="32"/>
       <c r="B36" s="26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>

</xml_diff>